<commit_message>
100pct with 5k data'
</commit_message>
<xml_diff>
--- a/oclog/openset/notebooks/trackerBKP4.xlsx
+++ b/oclog/openset/notebooks/trackerBKP4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhujay_ROG\MyDev\OCLog\oclog\openset\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F26392-AC56-4312-9F5F-44B38A986626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFFF8A8-C34D-4142-8640-933AAB1FBC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="684" windowWidth="21156" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21864" yWindow="348" windowWidth="24000" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
   <si>
     <t>ablation</t>
   </si>
@@ -308,6 +308,66 @@
   </si>
   <si>
     <t xml:space="preserve">more pre-training helped, lets increase the wait also </t>
+  </si>
+  <si>
+    <t>8.876045,8.88159,8.93639</t>
+  </si>
+  <si>
+    <t>data 3000</t>
+  </si>
+  <si>
+    <t>8.8898325,8.895605,8.950283</t>
+  </si>
+  <si>
+    <t>huge drop in score, lets increase the pretraining</t>
+  </si>
+  <si>
+    <t>8.883269,8.8890295,8.943727</t>
+  </si>
+  <si>
+    <t>increasing pre-training not helping, lets decrease</t>
+  </si>
+  <si>
+    <t>8.8833065,8.88892,8.943608</t>
+  </si>
+  <si>
+    <t>increasing pretraining a bit more</t>
+  </si>
+  <si>
+    <t>8.872322,8.87801,8.932601</t>
+  </si>
+  <si>
+    <t>training not increasing indicates learning probelm, lets increase em size</t>
+  </si>
+  <si>
+    <t>8.889619,8.89532,8.950037</t>
+  </si>
+  <si>
+    <t>em size increase by 2 did very good, what happens if we increase further</t>
+  </si>
+  <si>
+    <t>8.887793,8.89349,8.948126</t>
+  </si>
+  <si>
+    <t>em size 16 with 3000 99pct, now lets go for 4000 data</t>
+  </si>
+  <si>
+    <t>8.888987,8.894795</t>
+  </si>
+  <si>
+    <t>6.642053,6.647793</t>
+  </si>
+  <si>
+    <t>10000 data , more pre-training</t>
+  </si>
+  <si>
+    <t>8.890916,8.89661</t>
+  </si>
+  <si>
+    <t>5000 data , more pre-training</t>
+  </si>
+  <si>
+    <t>Oh 100 pct ! To be doubly sure</t>
   </si>
 </sst>
 </file>
@@ -331,7 +391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +401,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -381,6 +459,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +803,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1470,7 +1555,7 @@
       <c r="B15" s="3">
         <v>500</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>6</v>
       </c>
       <c r="D15" s="3">
@@ -1482,7 +1567,7 @@
       <c r="F15" s="3">
         <v>2</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="3">
@@ -2169,7 +2254,7 @@
       <c r="G27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="4">
         <v>16</v>
       </c>
       <c r="I27" s="3">
@@ -2455,7 +2540,7 @@
       <c r="D32" s="3">
         <v>3</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="4">
         <v>12</v>
       </c>
       <c r="F32" s="3">
@@ -2573,7 +2658,7 @@
       <c r="D34" s="3">
         <v>3</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="4">
         <v>12</v>
       </c>
       <c r="F34" s="3">
@@ -2625,7 +2710,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="4">
         <v>2000</v>
       </c>
       <c r="C35" s="3">
@@ -3174,7 +3259,7 @@
       <c r="G44" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="4">
         <v>10</v>
       </c>
       <c r="I44" s="3">
@@ -3270,7 +3355,725 @@
         <v>95</v>
       </c>
     </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>2500</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>2.6</v>
+      </c>
+      <c r="G46" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46">
+        <v>10</v>
+      </c>
+      <c r="I46">
+        <v>51</v>
+      </c>
+      <c r="J46">
+        <v>8</v>
+      </c>
+      <c r="K46">
+        <v>0.99218335732512486</v>
+      </c>
+      <c r="L46">
+        <v>99.100700000000003</v>
+      </c>
+      <c r="M46">
+        <v>99.523399999999995</v>
+      </c>
+      <c r="N46">
+        <v>97.832800000000006</v>
+      </c>
+      <c r="O46" t="s">
+        <v>55</v>
+      </c>
+      <c r="P46">
+        <v>535.03656005859375</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+      <c r="R46">
+        <v>1</v>
+      </c>
+      <c r="S46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <v>3000</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>12</v>
+      </c>
+      <c r="F47">
+        <v>2.6</v>
+      </c>
+      <c r="G47" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47">
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <v>31</v>
+      </c>
+      <c r="J47">
+        <v>8</v>
+      </c>
+      <c r="K47">
+        <v>0.64150432900432897</v>
+      </c>
+      <c r="L47">
+        <v>63.095199999999998</v>
+      </c>
+      <c r="M47">
+        <v>66.666700000000006</v>
+      </c>
+      <c r="N47">
+        <v>52.381</v>
+      </c>
+      <c r="O47" t="s">
+        <v>96</v>
+      </c>
+      <c r="P47">
+        <v>1609.544067382812</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>3000</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>12</v>
+      </c>
+      <c r="F48">
+        <v>2.6</v>
+      </c>
+      <c r="G48" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48">
+        <v>15</v>
+      </c>
+      <c r="I48">
+        <v>43</v>
+      </c>
+      <c r="J48">
+        <v>8</v>
+      </c>
+      <c r="K48">
+        <v>0.64150432900432897</v>
+      </c>
+      <c r="L48">
+        <v>63.095199999999998</v>
+      </c>
+      <c r="M48">
+        <v>66.666700000000006</v>
+      </c>
+      <c r="N48">
+        <v>52.381</v>
+      </c>
+      <c r="O48" t="s">
+        <v>98</v>
+      </c>
+      <c r="P48">
+        <v>1624.92578125</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+      <c r="S48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>3000</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <v>2.6</v>
+      </c>
+      <c r="G49" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49">
+        <v>3</v>
+      </c>
+      <c r="I49">
+        <v>34</v>
+      </c>
+      <c r="J49">
+        <v>8</v>
+      </c>
+      <c r="K49">
+        <v>0.92457573859581021</v>
+      </c>
+      <c r="L49">
+        <v>90.121300000000005</v>
+      </c>
+      <c r="M49">
+        <v>96.296599999999998</v>
+      </c>
+      <c r="N49">
+        <v>71.595299999999995</v>
+      </c>
+      <c r="O49" t="s">
+        <v>100</v>
+      </c>
+      <c r="P49">
+        <v>558.0235595703125</v>
+      </c>
+      <c r="Q49">
+        <v>0.99986112117767334</v>
+      </c>
+      <c r="R49">
+        <v>0.97991073131561279</v>
+      </c>
+      <c r="S49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>3000</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>2.6</v>
+      </c>
+      <c r="G50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>34</v>
+      </c>
+      <c r="J50">
+        <v>8</v>
+      </c>
+      <c r="K50">
+        <v>0.64150432900432897</v>
+      </c>
+      <c r="L50">
+        <v>63.095199999999998</v>
+      </c>
+      <c r="M50">
+        <v>66.666700000000006</v>
+      </c>
+      <c r="N50">
+        <v>52.381</v>
+      </c>
+      <c r="O50" t="s">
+        <v>102</v>
+      </c>
+      <c r="P50">
+        <v>1591.715698242188</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>48</v>
+      </c>
+      <c r="B51" s="3">
+        <v>3000</v>
+      </c>
+      <c r="C51" s="3">
+        <v>5</v>
+      </c>
+      <c r="D51" s="3">
+        <v>3</v>
+      </c>
+      <c r="E51" s="4">
+        <v>14</v>
+      </c>
+      <c r="F51" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H51" s="3">
+        <v>5</v>
+      </c>
+      <c r="I51" s="3">
+        <v>30</v>
+      </c>
+      <c r="J51" s="3">
+        <v>8</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0.98563334048871232</v>
+      </c>
+      <c r="L51" s="3">
+        <v>98.189700000000002</v>
+      </c>
+      <c r="M51" s="3">
+        <v>99.173599999999993</v>
+      </c>
+      <c r="N51" s="3">
+        <v>95.238100000000003</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P51" s="3">
+        <v>869.08892822265625</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>1</v>
+      </c>
+      <c r="R51" s="3">
+        <v>1</v>
+      </c>
+      <c r="S51" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>49</v>
+      </c>
+      <c r="B52" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C52" s="5">
+        <v>5</v>
+      </c>
+      <c r="D52" s="5">
+        <v>3</v>
+      </c>
+      <c r="E52" s="4">
+        <v>16</v>
+      </c>
+      <c r="F52" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H52" s="5">
+        <v>5</v>
+      </c>
+      <c r="I52" s="5">
+        <v>42</v>
+      </c>
+      <c r="J52" s="5">
+        <v>8</v>
+      </c>
+      <c r="K52" s="5">
+        <v>0.99905239199999996</v>
+      </c>
+      <c r="L52" s="5">
+        <v>99.881699999999995</v>
+      </c>
+      <c r="M52" s="5">
+        <v>99.943600000000004</v>
+      </c>
+      <c r="N52" s="5">
+        <v>99.695999999999998</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P52" s="5">
+        <v>1228.357178</v>
+      </c>
+      <c r="Q52" s="5">
+        <v>1</v>
+      </c>
+      <c r="R52" s="5">
+        <v>0.994419634</v>
+      </c>
+      <c r="S52" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="T52" s="5"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>50</v>
+      </c>
+      <c r="B53" s="7">
+        <v>4000</v>
+      </c>
+      <c r="C53" s="7">
+        <v>5</v>
+      </c>
+      <c r="D53" s="7">
+        <v>3</v>
+      </c>
+      <c r="E53" s="7">
+        <v>16</v>
+      </c>
+      <c r="F53" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" s="7">
+        <v>5</v>
+      </c>
+      <c r="I53" s="7">
+        <v>30</v>
+      </c>
+      <c r="J53" s="7">
+        <v>8</v>
+      </c>
+      <c r="K53" s="7">
+        <v>0.98685553195172082</v>
+      </c>
+      <c r="L53" s="7">
+        <v>98.111599999999996</v>
+      </c>
+      <c r="M53" s="7">
+        <v>99.226299999999995</v>
+      </c>
+      <c r="N53" s="7">
+        <v>94.767399999999995</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P53" s="7">
+        <v>1026.683715820312</v>
+      </c>
+      <c r="Q53" s="7">
+        <v>1</v>
+      </c>
+      <c r="R53" s="7">
+        <v>1</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>51</v>
+      </c>
+      <c r="B54" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>16</v>
+      </c>
+      <c r="F54">
+        <v>2.6</v>
+      </c>
+      <c r="G54" t="s">
+        <v>18</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54">
+        <v>37</v>
+      </c>
+      <c r="J54">
+        <v>8</v>
+      </c>
+      <c r="K54">
+        <v>0.99826028771874276</v>
+      </c>
+      <c r="L54">
+        <v>99.726799999999997</v>
+      </c>
+      <c r="M54">
+        <v>99.898799999999994</v>
+      </c>
+      <c r="N54">
+        <v>99.3827</v>
+      </c>
+      <c r="O54" t="s">
+        <v>110</v>
+      </c>
+      <c r="P54">
+        <v>744.86407470703125</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <v>5000</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>16</v>
+      </c>
+      <c r="F55">
+        <v>2.6</v>
+      </c>
+      <c r="G55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55">
+        <v>10</v>
+      </c>
+      <c r="I55">
+        <v>9</v>
+      </c>
+      <c r="J55">
+        <v>8</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>100</v>
+      </c>
+      <c r="M55">
+        <v>100</v>
+      </c>
+      <c r="N55">
+        <v>100</v>
+      </c>
+      <c r="O55" t="s">
+        <v>111</v>
+      </c>
+      <c r="P55">
+        <v>772.7252197265625</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+      <c r="S55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>53</v>
+      </c>
+      <c r="B56" s="7">
+        <v>5000</v>
+      </c>
+      <c r="C56" s="7">
+        <v>5</v>
+      </c>
+      <c r="D56" s="7">
+        <v>2</v>
+      </c>
+      <c r="E56" s="7">
+        <v>16</v>
+      </c>
+      <c r="F56" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" s="4">
+        <v>10</v>
+      </c>
+      <c r="I56" s="7">
+        <v>9</v>
+      </c>
+      <c r="J56" s="7">
+        <v>8</v>
+      </c>
+      <c r="K56" s="7">
+        <v>1</v>
+      </c>
+      <c r="L56" s="7">
+        <v>100</v>
+      </c>
+      <c r="M56" s="7">
+        <v>100</v>
+      </c>
+      <c r="N56" s="7">
+        <v>100</v>
+      </c>
+      <c r="O56" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="P56" s="7">
+        <v>772.7252197265625</v>
+      </c>
+      <c r="Q56" s="7">
+        <v>1</v>
+      </c>
+      <c r="R56" s="7">
+        <v>1</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>10000</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>16</v>
+      </c>
+      <c r="F57">
+        <v>2.6</v>
+      </c>
+      <c r="G57" t="s">
+        <v>18</v>
+      </c>
+      <c r="H57">
+        <v>10</v>
+      </c>
+      <c r="I57">
+        <v>39</v>
+      </c>
+      <c r="J57">
+        <v>8</v>
+      </c>
+      <c r="K57">
+        <v>0.48940896592344901</v>
+      </c>
+      <c r="L57">
+        <v>41.771900000000002</v>
+      </c>
+      <c r="M57">
+        <v>51.076000000000001</v>
+      </c>
+      <c r="N57">
+        <v>23.163799999999998</v>
+      </c>
+      <c r="O57" t="s">
+        <v>113</v>
+      </c>
+      <c r="P57">
+        <v>6117.12890625</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
+      <c r="S57" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
99known-94open pct with 10K data'
</commit_message>
<xml_diff>
--- a/oclog/openset/notebooks/trackerBKP4.xlsx
+++ b/oclog/openset/notebooks/trackerBKP4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhujay_ROG\MyDev\OCLog\oclog\openset\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFFF8A8-C34D-4142-8640-933AAB1FBC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C0D1F1-B734-4039-A4F7-F9A04E840664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21864" yWindow="348" windowWidth="24000" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="456" yWindow="396" windowWidth="24000" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="162">
   <si>
     <t>ablation</t>
   </si>
@@ -368,6 +368,144 @@
   </si>
   <si>
     <t>Oh 100 pct ! To be doubly sure</t>
+  </si>
+  <si>
+    <t>8.888643,8.894331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increase emsize a bit </t>
+  </si>
+  <si>
+    <t>8.845131,8.850864</t>
+  </si>
+  <si>
+    <t>increase emsize more</t>
+  </si>
+  <si>
+    <t>8.890071,8.895768</t>
+  </si>
+  <si>
+    <t>8.874122,8.879835</t>
+  </si>
+  <si>
+    <t>8.8807535,8.886441</t>
+  </si>
+  <si>
+    <t>increase data more</t>
+  </si>
+  <si>
+    <t>8.890586,8.896346</t>
+  </si>
+  <si>
+    <t>increase emsize a bit with 20K</t>
+  </si>
+  <si>
+    <t>8.880667,8.886354</t>
+  </si>
+  <si>
+    <t>increase emsize more with 20K</t>
+  </si>
+  <si>
+    <t>8.887132,8.892819</t>
+  </si>
+  <si>
+    <t>increase pretrain with 20K</t>
+  </si>
+  <si>
+    <t>8.880751,8.886431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emsize more </t>
+  </si>
+  <si>
+    <t>8.863184,8.868924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduce pretraining </t>
+  </si>
+  <si>
+    <t>8.890098,8.895679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre-training not helping, lets try em-size reduction </t>
+  </si>
+  <si>
+    <t>8.815405,8.821115</t>
+  </si>
+  <si>
+    <t>8.81509,8.820725</t>
+  </si>
+  <si>
+    <t>8.683181,8.6888685</t>
+  </si>
+  <si>
+    <t>reduce em size and increase pre -train</t>
+  </si>
+  <si>
+    <t>8.880718,8.8864155</t>
+  </si>
+  <si>
+    <t>decrease pretrain with 20K</t>
+  </si>
+  <si>
+    <t>8.880511,8.886233</t>
+  </si>
+  <si>
+    <t>8.188752,8.194465</t>
+  </si>
+  <si>
+    <t>restore best score setting and reduce lr</t>
+  </si>
+  <si>
+    <t>9.493434,9.499144</t>
+  </si>
+  <si>
+    <t>10.694959,10.700581</t>
+  </si>
+  <si>
+    <t>10.788132,10.793786</t>
+  </si>
+  <si>
+    <t>increase em size wiht increased lr</t>
+  </si>
+  <si>
+    <t>13.314365,13.319825</t>
+  </si>
+  <si>
+    <t>13.201913,13.2075815</t>
+  </si>
+  <si>
+    <t>increasing lr helped, increase em size a bit</t>
+  </si>
+  <si>
+    <t>14.888033,14.892715</t>
+  </si>
+  <si>
+    <t>16.426922,16.432648</t>
+  </si>
+  <si>
+    <t>increasing lr is helping, lets increse more</t>
+  </si>
+  <si>
+    <t>15.197124,15.202749</t>
+  </si>
+  <si>
+    <t>although score for known improved, open score dropped, lets decrease a bit</t>
+  </si>
+  <si>
+    <t>14.851324,14.857045</t>
+  </si>
+  <si>
+    <t>increase the data to 20K</t>
+  </si>
+  <si>
+    <t>16.460815,16.466543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lr is not helping, class-1 is getting misclassified, we have to improve pretrain validation  </t>
+  </si>
+  <si>
+    <t>16.479412,16.485113</t>
   </si>
 </sst>
 </file>
@@ -391,7 +529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +557,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -465,6 +615,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,11 +960,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W57"/>
+  <dimension ref="A1:W92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S81" sqref="S81:S82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4072,6 +4229,1690 @@
         <v>112</v>
       </c>
     </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>10000</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>18</v>
+      </c>
+      <c r="F58">
+        <v>2.6</v>
+      </c>
+      <c r="G58" t="s">
+        <v>18</v>
+      </c>
+      <c r="H58">
+        <v>10</v>
+      </c>
+      <c r="I58">
+        <v>21</v>
+      </c>
+      <c r="J58">
+        <v>8</v>
+      </c>
+      <c r="K58">
+        <v>0.74461299076706888</v>
+      </c>
+      <c r="L58">
+        <v>63.436300000000003</v>
+      </c>
+      <c r="M58">
+        <v>77.744799999999998</v>
+      </c>
+      <c r="N58">
+        <v>34.819499999999998</v>
+      </c>
+      <c r="O58" t="s">
+        <v>116</v>
+      </c>
+      <c r="P58">
+        <v>3336.19482421875</v>
+      </c>
+      <c r="Q58">
+        <v>1</v>
+      </c>
+      <c r="R58">
+        <v>1</v>
+      </c>
+      <c r="S58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <v>10000</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>20</v>
+      </c>
+      <c r="F59">
+        <v>2.6</v>
+      </c>
+      <c r="G59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59">
+        <v>10</v>
+      </c>
+      <c r="I59">
+        <v>15</v>
+      </c>
+      <c r="J59">
+        <v>8</v>
+      </c>
+      <c r="K59">
+        <v>0.7680202776746371</v>
+      </c>
+      <c r="L59">
+        <v>65.634600000000006</v>
+      </c>
+      <c r="M59">
+        <v>80.127899999999997</v>
+      </c>
+      <c r="N59">
+        <v>36.648000000000003</v>
+      </c>
+      <c r="O59" t="s">
+        <v>118</v>
+      </c>
+      <c r="P59">
+        <v>2216.86572265625</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+      <c r="S59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <v>10000</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>22</v>
+      </c>
+      <c r="F60">
+        <v>2.6</v>
+      </c>
+      <c r="G60" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60">
+        <v>10</v>
+      </c>
+      <c r="I60">
+        <v>23</v>
+      </c>
+      <c r="J60">
+        <v>8</v>
+      </c>
+      <c r="K60">
+        <v>0.7676474233559667</v>
+      </c>
+      <c r="L60">
+        <v>65.556899999999999</v>
+      </c>
+      <c r="M60">
+        <v>80.102699999999999</v>
+      </c>
+      <c r="N60">
+        <v>36.465299999999999</v>
+      </c>
+      <c r="O60" t="s">
+        <v>120</v>
+      </c>
+      <c r="P60">
+        <v>1946.071899414062</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+      <c r="R60">
+        <v>1</v>
+      </c>
+      <c r="S60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <v>10000</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>22</v>
+      </c>
+      <c r="F61">
+        <v>2.6</v>
+      </c>
+      <c r="G61" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61">
+        <v>15</v>
+      </c>
+      <c r="I61">
+        <v>17</v>
+      </c>
+      <c r="J61">
+        <v>8</v>
+      </c>
+      <c r="K61">
+        <v>0.7680202776746371</v>
+      </c>
+      <c r="L61">
+        <v>65.634600000000006</v>
+      </c>
+      <c r="M61">
+        <v>80.127899999999997</v>
+      </c>
+      <c r="N61">
+        <v>36.648000000000003</v>
+      </c>
+      <c r="O61" t="s">
+        <v>121</v>
+      </c>
+      <c r="P61">
+        <v>2073.2880859375</v>
+      </c>
+      <c r="Q61">
+        <v>1</v>
+      </c>
+      <c r="R61">
+        <v>1</v>
+      </c>
+      <c r="S61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62">
+        <v>10000</v>
+      </c>
+      <c r="C62">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>22</v>
+      </c>
+      <c r="F62">
+        <v>2.6</v>
+      </c>
+      <c r="G62" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62">
+        <v>15</v>
+      </c>
+      <c r="I62">
+        <v>18</v>
+      </c>
+      <c r="J62">
+        <v>8</v>
+      </c>
+      <c r="K62">
+        <v>0.7680202776746371</v>
+      </c>
+      <c r="L62">
+        <v>65.634600000000006</v>
+      </c>
+      <c r="M62">
+        <v>80.127899999999997</v>
+      </c>
+      <c r="N62">
+        <v>36.648000000000003</v>
+      </c>
+      <c r="O62" t="s">
+        <v>130</v>
+      </c>
+      <c r="P62">
+        <v>2076.974365234375</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63">
+        <v>10000</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>22</v>
+      </c>
+      <c r="F63">
+        <v>2.6</v>
+      </c>
+      <c r="G63" t="s">
+        <v>18</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63">
+        <v>16</v>
+      </c>
+      <c r="J63">
+        <v>8</v>
+      </c>
+      <c r="K63">
+        <v>0.7676474233559667</v>
+      </c>
+      <c r="L63">
+        <v>65.556899999999999</v>
+      </c>
+      <c r="M63">
+        <v>80.102699999999999</v>
+      </c>
+      <c r="N63">
+        <v>36.465299999999999</v>
+      </c>
+      <c r="O63" t="s">
+        <v>132</v>
+      </c>
+      <c r="P63">
+        <v>1803.791137695312</v>
+      </c>
+      <c r="Q63">
+        <v>1</v>
+      </c>
+      <c r="R63">
+        <v>1</v>
+      </c>
+      <c r="S63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64">
+        <v>10000</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>16</v>
+      </c>
+      <c r="F64">
+        <v>2.6</v>
+      </c>
+      <c r="G64" t="s">
+        <v>18</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64">
+        <v>24</v>
+      </c>
+      <c r="J64">
+        <v>8</v>
+      </c>
+      <c r="K64">
+        <v>0.7680202776746371</v>
+      </c>
+      <c r="L64">
+        <v>65.634600000000006</v>
+      </c>
+      <c r="M64">
+        <v>80.127899999999997</v>
+      </c>
+      <c r="N64">
+        <v>36.648000000000003</v>
+      </c>
+      <c r="O64" t="s">
+        <v>134</v>
+      </c>
+      <c r="P64">
+        <v>2998.32861328125</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
+      </c>
+      <c r="R64">
+        <v>1</v>
+      </c>
+      <c r="S64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65">
+        <v>10000</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>16</v>
+      </c>
+      <c r="F65">
+        <v>2.6</v>
+      </c>
+      <c r="G65" t="s">
+        <v>18</v>
+      </c>
+      <c r="H65">
+        <v>10</v>
+      </c>
+      <c r="I65">
+        <v>14</v>
+      </c>
+      <c r="J65">
+        <v>8</v>
+      </c>
+      <c r="K65">
+        <v>0.77426624452258919</v>
+      </c>
+      <c r="L65">
+        <v>66.235699999999994</v>
+      </c>
+      <c r="M65">
+        <v>80.759500000000003</v>
+      </c>
+      <c r="N65">
+        <v>37.188200000000002</v>
+      </c>
+      <c r="O65" t="s">
+        <v>136</v>
+      </c>
+      <c r="P65">
+        <v>2348.560791015625</v>
+      </c>
+      <c r="Q65">
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <v>1</v>
+      </c>
+      <c r="S65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66">
+        <v>10000</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66" s="3">
+        <v>14</v>
+      </c>
+      <c r="F66">
+        <v>2.6</v>
+      </c>
+      <c r="G66" t="s">
+        <v>18</v>
+      </c>
+      <c r="H66" s="3">
+        <v>15</v>
+      </c>
+      <c r="I66">
+        <v>14</v>
+      </c>
+      <c r="J66">
+        <v>8</v>
+      </c>
+      <c r="K66">
+        <v>0.77474283126089427</v>
+      </c>
+      <c r="L66">
+        <v>66.281899999999993</v>
+      </c>
+      <c r="M66">
+        <v>80.807599999999994</v>
+      </c>
+      <c r="N66">
+        <v>37.230400000000003</v>
+      </c>
+      <c r="O66" t="s">
+        <v>137</v>
+      </c>
+      <c r="P66">
+        <v>1728.87451171875</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <v>1</v>
+      </c>
+      <c r="S66" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67">
+        <v>10000</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>12</v>
+      </c>
+      <c r="F67">
+        <v>2.6</v>
+      </c>
+      <c r="G67" t="s">
+        <v>18</v>
+      </c>
+      <c r="H67">
+        <v>20</v>
+      </c>
+      <c r="I67">
+        <v>12</v>
+      </c>
+      <c r="J67">
+        <v>8</v>
+      </c>
+      <c r="K67">
+        <v>0.76727449216536481</v>
+      </c>
+      <c r="L67">
+        <v>65.478999999999999</v>
+      </c>
+      <c r="M67">
+        <v>80.077500000000001</v>
+      </c>
+      <c r="N67">
+        <v>36.282200000000003</v>
+      </c>
+      <c r="O67" t="s">
+        <v>138</v>
+      </c>
+      <c r="P67">
+        <v>1776.686767578125</v>
+      </c>
+      <c r="Q67">
+        <v>1</v>
+      </c>
+      <c r="R67">
+        <v>1</v>
+      </c>
+      <c r="S67" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68">
+        <v>10000</v>
+      </c>
+      <c r="C68">
+        <v>5</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>22</v>
+      </c>
+      <c r="F68">
+        <v>2.4</v>
+      </c>
+      <c r="G68" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68">
+        <v>20</v>
+      </c>
+      <c r="I68">
+        <v>14</v>
+      </c>
+      <c r="J68">
+        <v>8</v>
+      </c>
+      <c r="K68">
+        <v>0.76775376658552641</v>
+      </c>
+      <c r="L68">
+        <v>65.603999999999999</v>
+      </c>
+      <c r="M68">
+        <v>80.102400000000003</v>
+      </c>
+      <c r="N68">
+        <v>36.607100000000003</v>
+      </c>
+      <c r="O68" t="s">
+        <v>143</v>
+      </c>
+      <c r="P68">
+        <v>2204.143310546875</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
+      <c r="S68" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69">
+        <v>10000</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>14</v>
+      </c>
+      <c r="F69">
+        <v>2.8</v>
+      </c>
+      <c r="G69" t="s">
+        <v>18</v>
+      </c>
+      <c r="H69">
+        <v>15</v>
+      </c>
+      <c r="I69">
+        <v>16</v>
+      </c>
+      <c r="J69">
+        <v>8</v>
+      </c>
+      <c r="K69">
+        <v>0.81946631203647546</v>
+      </c>
+      <c r="L69">
+        <v>70.821200000000005</v>
+      </c>
+      <c r="M69">
+        <v>85.26</v>
+      </c>
+      <c r="N69">
+        <v>41.9437</v>
+      </c>
+      <c r="O69" t="s">
+        <v>145</v>
+      </c>
+      <c r="P69">
+        <v>1728.853149414062</v>
+      </c>
+      <c r="Q69">
+        <v>1</v>
+      </c>
+      <c r="R69">
+        <v>1</v>
+      </c>
+      <c r="S69" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70">
+        <v>10000</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>14</v>
+      </c>
+      <c r="F70">
+        <v>3.2</v>
+      </c>
+      <c r="G70" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70">
+        <v>15</v>
+      </c>
+      <c r="I70">
+        <v>14</v>
+      </c>
+      <c r="J70">
+        <v>8</v>
+      </c>
+      <c r="K70">
+        <v>0.82966324429865268</v>
+      </c>
+      <c r="L70">
+        <v>71.926699999999997</v>
+      </c>
+      <c r="M70">
+        <v>86.254199999999997</v>
+      </c>
+      <c r="N70">
+        <v>43.271799999999999</v>
+      </c>
+      <c r="O70" t="s">
+        <v>146</v>
+      </c>
+      <c r="P70">
+        <v>1728.86572265625</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
+      </c>
+      <c r="R70">
+        <v>1</v>
+      </c>
+      <c r="S70" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71">
+        <v>10000</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>16</v>
+      </c>
+      <c r="F71">
+        <v>3.2</v>
+      </c>
+      <c r="G71" t="s">
+        <v>18</v>
+      </c>
+      <c r="H71">
+        <v>15</v>
+      </c>
+      <c r="I71">
+        <v>27</v>
+      </c>
+      <c r="J71">
+        <v>8</v>
+      </c>
+      <c r="K71">
+        <v>0.7680202776746371</v>
+      </c>
+      <c r="L71">
+        <v>65.634600000000006</v>
+      </c>
+      <c r="M71">
+        <v>80.127899999999997</v>
+      </c>
+      <c r="N71">
+        <v>36.648000000000003</v>
+      </c>
+      <c r="O71" t="s">
+        <v>147</v>
+      </c>
+      <c r="P71">
+        <v>3279.3408203125</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
+      </c>
+      <c r="R71">
+        <v>1</v>
+      </c>
+      <c r="S71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72">
+        <v>10000</v>
+      </c>
+      <c r="C72">
+        <v>5</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>14</v>
+      </c>
+      <c r="F72">
+        <v>4</v>
+      </c>
+      <c r="G72" t="s">
+        <v>18</v>
+      </c>
+      <c r="H72">
+        <v>15</v>
+      </c>
+      <c r="I72">
+        <v>21</v>
+      </c>
+      <c r="J72">
+        <v>8</v>
+      </c>
+      <c r="K72">
+        <v>0.94328131699546824</v>
+      </c>
+      <c r="L72">
+        <v>87.640600000000006</v>
+      </c>
+      <c r="M72">
+        <v>96.319800000000001</v>
+      </c>
+      <c r="N72">
+        <v>70.281999999999996</v>
+      </c>
+      <c r="O72" t="s">
+        <v>149</v>
+      </c>
+      <c r="P72">
+        <v>1728.8349609375</v>
+      </c>
+      <c r="Q72">
+        <v>1</v>
+      </c>
+      <c r="R72">
+        <v>1</v>
+      </c>
+      <c r="S72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73">
+        <v>10000</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>16</v>
+      </c>
+      <c r="F73">
+        <v>4</v>
+      </c>
+      <c r="G73" t="s">
+        <v>18</v>
+      </c>
+      <c r="H73">
+        <v>15</v>
+      </c>
+      <c r="I73">
+        <v>14</v>
+      </c>
+      <c r="J73">
+        <v>8</v>
+      </c>
+      <c r="K73">
+        <v>0.76727449216536481</v>
+      </c>
+      <c r="L73">
+        <v>65.478999999999999</v>
+      </c>
+      <c r="M73">
+        <v>80.077500000000001</v>
+      </c>
+      <c r="N73">
+        <v>36.282200000000003</v>
+      </c>
+      <c r="O73" t="s">
+        <v>150</v>
+      </c>
+      <c r="P73">
+        <v>3279.37060546875</v>
+      </c>
+      <c r="Q73">
+        <v>1</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+      <c r="S73" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="8"/>
+      <c r="B74" s="9">
+        <v>10000</v>
+      </c>
+      <c r="C74" s="9">
+        <v>5</v>
+      </c>
+      <c r="D74" s="9">
+        <v>2</v>
+      </c>
+      <c r="E74" s="9">
+        <v>14</v>
+      </c>
+      <c r="F74" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H74" s="9">
+        <v>15</v>
+      </c>
+      <c r="I74" s="9">
+        <v>19</v>
+      </c>
+      <c r="J74" s="9">
+        <v>8</v>
+      </c>
+      <c r="K74" s="9">
+        <v>0.99203653615203247</v>
+      </c>
+      <c r="L74" s="9">
+        <v>97.970399999999998</v>
+      </c>
+      <c r="M74" s="10">
+        <v>99.570899999999995</v>
+      </c>
+      <c r="N74" s="10">
+        <v>94.769199999999998</v>
+      </c>
+      <c r="O74" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="P74" s="9">
+        <v>1728.854370117188</v>
+      </c>
+      <c r="Q74" s="9">
+        <v>1</v>
+      </c>
+      <c r="R74" s="9">
+        <v>1</v>
+      </c>
+      <c r="S74" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75">
+        <v>10000</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>14</v>
+      </c>
+      <c r="F75">
+        <v>5</v>
+      </c>
+      <c r="G75" t="s">
+        <v>18</v>
+      </c>
+      <c r="H75">
+        <v>15</v>
+      </c>
+      <c r="I75">
+        <v>16</v>
+      </c>
+      <c r="J75">
+        <v>8</v>
+      </c>
+      <c r="K75">
+        <v>0.98435066615243916</v>
+      </c>
+      <c r="L75">
+        <v>95.863699999999994</v>
+      </c>
+      <c r="M75">
+        <v>99.200900000000004</v>
+      </c>
+      <c r="N75">
+        <v>89.1892</v>
+      </c>
+      <c r="O75" t="s">
+        <v>153</v>
+      </c>
+      <c r="P75">
+        <v>1728.84521484375</v>
+      </c>
+      <c r="Q75">
+        <v>1</v>
+      </c>
+      <c r="R75">
+        <v>1</v>
+      </c>
+      <c r="S75" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76">
+        <v>10000</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>14</v>
+      </c>
+      <c r="F76">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G76" t="s">
+        <v>18</v>
+      </c>
+      <c r="H76">
+        <v>15</v>
+      </c>
+      <c r="I76">
+        <v>18</v>
+      </c>
+      <c r="J76">
+        <v>8</v>
+      </c>
+      <c r="K76">
+        <v>0.99155547767935093</v>
+      </c>
+      <c r="L76">
+        <v>97.845299999999995</v>
+      </c>
+      <c r="M76">
+        <v>99.5458</v>
+      </c>
+      <c r="N76">
+        <v>94.444400000000002</v>
+      </c>
+      <c r="O76" t="s">
+        <v>155</v>
+      </c>
+      <c r="P76">
+        <v>1728.877563476562</v>
+      </c>
+      <c r="Q76">
+        <v>1</v>
+      </c>
+      <c r="R76">
+        <v>1</v>
+      </c>
+      <c r="S76" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C77" s="11">
+        <v>5</v>
+      </c>
+      <c r="D77" s="11">
+        <v>2</v>
+      </c>
+      <c r="E77" s="11">
+        <v>14</v>
+      </c>
+      <c r="F77" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H77" s="11">
+        <v>15</v>
+      </c>
+      <c r="I77" s="11">
+        <v>11</v>
+      </c>
+      <c r="J77" s="11">
+        <v>8</v>
+      </c>
+      <c r="K77" s="11">
+        <v>0.55925198124638698</v>
+      </c>
+      <c r="L77" s="11">
+        <v>43.493699999999997</v>
+      </c>
+      <c r="M77" s="11">
+        <v>57.6158</v>
+      </c>
+      <c r="N77" s="11">
+        <v>15.249499999999999</v>
+      </c>
+      <c r="O77" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P77" s="11">
+        <v>5583.88671875</v>
+      </c>
+      <c r="Q77" s="11">
+        <v>1</v>
+      </c>
+      <c r="R77" s="11">
+        <v>0.96899998188018799</v>
+      </c>
+      <c r="S77" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="12">
+        <v>20000</v>
+      </c>
+      <c r="C78" s="12">
+        <v>5</v>
+      </c>
+      <c r="D78" s="12">
+        <v>2</v>
+      </c>
+      <c r="E78" s="12">
+        <v>10</v>
+      </c>
+      <c r="F78" s="12">
+        <v>5</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" s="12">
+        <v>5</v>
+      </c>
+      <c r="I78" s="12">
+        <v>12</v>
+      </c>
+      <c r="J78" s="12">
+        <v>8</v>
+      </c>
+      <c r="K78" s="12">
+        <v>0.7261960640365257</v>
+      </c>
+      <c r="L78" s="12">
+        <v>56.248600000000003</v>
+      </c>
+      <c r="M78" s="12">
+        <v>74.837599999999995</v>
+      </c>
+      <c r="N78" s="12">
+        <v>19.070599999999999</v>
+      </c>
+      <c r="O78" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="P78" s="12">
+        <v>4444.0791015625</v>
+      </c>
+      <c r="Q78" s="12">
+        <v>1</v>
+      </c>
+      <c r="R78" s="12">
+        <v>0.98075002431869507</v>
+      </c>
+      <c r="S78" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79">
+        <v>20000</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>8</v>
+      </c>
+      <c r="F79">
+        <v>5</v>
+      </c>
+      <c r="G79" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79">
+        <v>8</v>
+      </c>
+      <c r="I79">
+        <v>15</v>
+      </c>
+      <c r="J79">
+        <v>8</v>
+      </c>
+      <c r="K79">
+        <v>0.554268549</v>
+      </c>
+      <c r="L79">
+        <v>43.122100000000003</v>
+      </c>
+      <c r="M79">
+        <v>57.1004</v>
+      </c>
+      <c r="N79">
+        <v>15.1654</v>
+      </c>
+      <c r="O79" t="s">
+        <v>161</v>
+      </c>
+      <c r="P79">
+        <v>10900.84375</v>
+      </c>
+      <c r="Q79">
+        <v>1</v>
+      </c>
+      <c r="R79">
+        <v>0.98750001200000004</v>
+      </c>
+      <c r="S79" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>59</v>
+      </c>
+      <c r="B86">
+        <v>20000</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86">
+        <v>22</v>
+      </c>
+      <c r="F86">
+        <v>2.6</v>
+      </c>
+      <c r="G86" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86">
+        <v>15</v>
+      </c>
+      <c r="I86">
+        <v>12</v>
+      </c>
+      <c r="J86">
+        <v>8</v>
+      </c>
+      <c r="K86">
+        <v>0.64874958621940393</v>
+      </c>
+      <c r="L86">
+        <v>50.289499999999997</v>
+      </c>
+      <c r="M86">
+        <v>66.853899999999996</v>
+      </c>
+      <c r="N86">
+        <v>17.160699999999999</v>
+      </c>
+      <c r="O86" t="s">
+        <v>122</v>
+      </c>
+      <c r="P86">
+        <v>2682.439208984375</v>
+      </c>
+      <c r="Q86">
+        <v>1</v>
+      </c>
+      <c r="R86">
+        <v>0.98849999904632568</v>
+      </c>
+      <c r="S86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>60</v>
+      </c>
+      <c r="B87">
+        <v>20000</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>24</v>
+      </c>
+      <c r="F87">
+        <v>2.6</v>
+      </c>
+      <c r="G87" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87">
+        <v>15</v>
+      </c>
+      <c r="I87">
+        <v>17</v>
+      </c>
+      <c r="J87">
+        <v>8</v>
+      </c>
+      <c r="K87">
+        <v>0.6906237801432944</v>
+      </c>
+      <c r="L87">
+        <v>53.275199999999998</v>
+      </c>
+      <c r="M87">
+        <v>71.202399999999997</v>
+      </c>
+      <c r="N87">
+        <v>17.4208</v>
+      </c>
+      <c r="O87" t="s">
+        <v>124</v>
+      </c>
+      <c r="P87">
+        <v>2159.773193359375</v>
+      </c>
+      <c r="Q87">
+        <v>1</v>
+      </c>
+      <c r="R87">
+        <v>0.97699999809265137</v>
+      </c>
+      <c r="S87" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>61</v>
+      </c>
+      <c r="B88">
+        <v>20000</v>
+      </c>
+      <c r="C88">
+        <v>5</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>28</v>
+      </c>
+      <c r="F88">
+        <v>2.6</v>
+      </c>
+      <c r="G88" t="s">
+        <v>18</v>
+      </c>
+      <c r="H88">
+        <v>15</v>
+      </c>
+      <c r="I88">
+        <v>12</v>
+      </c>
+      <c r="J88">
+        <v>8</v>
+      </c>
+      <c r="K88">
+        <v>0.56143537966578438</v>
+      </c>
+      <c r="L88">
+        <v>43.658200000000001</v>
+      </c>
+      <c r="M88">
+        <v>57.841299999999997</v>
+      </c>
+      <c r="N88">
+        <v>15.2919</v>
+      </c>
+      <c r="O88" t="s">
+        <v>126</v>
+      </c>
+      <c r="P88">
+        <v>4147.435546875</v>
+      </c>
+      <c r="Q88">
+        <v>1</v>
+      </c>
+      <c r="R88">
+        <v>0.95499998331069946</v>
+      </c>
+      <c r="S88" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>62</v>
+      </c>
+      <c r="B89">
+        <v>20000</v>
+      </c>
+      <c r="C89">
+        <v>5</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <v>28</v>
+      </c>
+      <c r="F89">
+        <v>2.6</v>
+      </c>
+      <c r="G89" t="s">
+        <v>18</v>
+      </c>
+      <c r="H89">
+        <v>20</v>
+      </c>
+      <c r="I89">
+        <v>13</v>
+      </c>
+      <c r="J89">
+        <v>8</v>
+      </c>
+      <c r="K89">
+        <v>0.55771991849542768</v>
+      </c>
+      <c r="L89">
+        <v>43.380899999999997</v>
+      </c>
+      <c r="M89">
+        <v>57.4572</v>
+      </c>
+      <c r="N89">
+        <v>15.228400000000001</v>
+      </c>
+      <c r="O89" t="s">
+        <v>128</v>
+      </c>
+      <c r="P89">
+        <v>4350.97900390625</v>
+      </c>
+      <c r="Q89">
+        <v>1</v>
+      </c>
+      <c r="R89">
+        <v>0.95499998331069946</v>
+      </c>
+      <c r="S89" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>20000</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>28</v>
+      </c>
+      <c r="F90">
+        <v>2.6</v>
+      </c>
+      <c r="G90" t="s">
+        <v>18</v>
+      </c>
+      <c r="H90">
+        <v>10</v>
+      </c>
+      <c r="I90">
+        <v>12</v>
+      </c>
+      <c r="J90">
+        <v>8</v>
+      </c>
+      <c r="K90">
+        <v>0.56552814805179585</v>
+      </c>
+      <c r="L90">
+        <v>43.963999999999999</v>
+      </c>
+      <c r="M90">
+        <v>58.264499999999998</v>
+      </c>
+      <c r="N90">
+        <v>15.363099999999999</v>
+      </c>
+      <c r="O90" t="s">
+        <v>140</v>
+      </c>
+      <c r="P90">
+        <v>3986.552734375</v>
+      </c>
+      <c r="Q90">
+        <v>1</v>
+      </c>
+      <c r="R90">
+        <v>0.95499998331069946</v>
+      </c>
+      <c r="S90" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>20000</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>16</v>
+      </c>
+      <c r="F91">
+        <v>2.6</v>
+      </c>
+      <c r="G91" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91">
+        <v>10</v>
+      </c>
+      <c r="I91">
+        <v>12</v>
+      </c>
+      <c r="J91">
+        <v>8</v>
+      </c>
+      <c r="K91">
+        <v>0.68741226312015269</v>
+      </c>
+      <c r="L91">
+        <v>53.132599999999996</v>
+      </c>
+      <c r="M91">
+        <v>70.857299999999995</v>
+      </c>
+      <c r="N91">
+        <v>17.683299999999999</v>
+      </c>
+      <c r="O91" t="s">
+        <v>142</v>
+      </c>
+      <c r="P91">
+        <v>1850.370361328125</v>
+      </c>
+      <c r="Q91">
+        <v>1</v>
+      </c>
+      <c r="R91">
+        <v>0.97675001621246338</v>
+      </c>
+      <c r="S91" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>20000</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>16</v>
+      </c>
+      <c r="F92">
+        <v>2.6</v>
+      </c>
+      <c r="G92" t="s">
+        <v>18</v>
+      </c>
+      <c r="H92">
+        <v>10</v>
+      </c>
+      <c r="I92">
+        <v>12</v>
+      </c>
+      <c r="J92">
+        <v>8</v>
+      </c>
+      <c r="K92">
+        <v>0.68741226312015269</v>
+      </c>
+      <c r="L92">
+        <v>53.132599999999996</v>
+      </c>
+      <c r="M92">
+        <v>70.857299999999995</v>
+      </c>
+      <c r="N92">
+        <v>17.683299999999999</v>
+      </c>
+      <c r="O92" t="s">
+        <v>142</v>
+      </c>
+      <c r="P92">
+        <v>1850.370361328125</v>
+      </c>
+      <c r="Q92">
+        <v>1</v>
+      </c>
+      <c r="R92">
+        <v>0.97675001621246338</v>
+      </c>
+      <c r="S92" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tsne for 5k and 1.5k to show the difference
</commit_message>
<xml_diff>
--- a/oclog/openset/notebooks/trackerBKP4.xlsx
+++ b/oclog/openset/notebooks/trackerBKP4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhujay_ROG\MyDev\OCLog\oclog\openset\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4286052-104B-4AE6-8F3E-EEC56CE96235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E276CB1-4964-4EFE-8FBE-CB003DB07E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="108" yWindow="360" windowWidth="23016" windowHeight="17604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1236" yWindow="936" windowWidth="24540" windowHeight="17604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="242">
   <si>
     <t>ablation</t>
   </si>
@@ -743,6 +743,9 @@
   </si>
   <si>
     <t>15.531617,15.537371</t>
+  </si>
+  <si>
+    <t>Mixed-176</t>
   </si>
 </sst>
 </file>
@@ -974,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1103,6 +1106,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1442,11 +1472,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE134"/>
+  <dimension ref="A1:AE139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M140" sqref="M140"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8381,161 +8411,161 @@
         <v>231</v>
       </c>
     </row>
-    <row r="110" spans="1:30" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="32">
-        <v>64</v>
-      </c>
-      <c r="B110" s="33">
+    <row r="110" spans="1:30" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="58">
+        <v>64</v>
+      </c>
+      <c r="B110" s="59">
         <v>18000</v>
       </c>
-      <c r="C110" s="34">
+      <c r="C110" s="60">
         <v>0.98</v>
       </c>
-      <c r="D110" s="34">
+      <c r="D110" s="60">
         <v>32</v>
       </c>
-      <c r="E110" s="34">
-        <v>5</v>
-      </c>
-      <c r="F110" s="34">
-        <v>2</v>
-      </c>
-      <c r="G110" s="34">
+      <c r="E110" s="60">
+        <v>5</v>
+      </c>
+      <c r="F110" s="60">
+        <v>2</v>
+      </c>
+      <c r="G110" s="60">
         <v>14</v>
       </c>
-      <c r="H110" s="34">
+      <c r="H110" s="60">
         <v>4.7</v>
       </c>
-      <c r="I110" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="J110" s="34">
+      <c r="I110" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J110" s="60">
         <v>15</v>
       </c>
-      <c r="K110" s="34">
+      <c r="K110" s="60">
         <v>15</v>
       </c>
-      <c r="L110" s="34">
-        <v>8</v>
-      </c>
-      <c r="M110" s="34">
+      <c r="L110" s="60">
+        <v>8</v>
+      </c>
+      <c r="M110" s="60">
         <v>0.61397998980000001</v>
       </c>
-      <c r="N110" s="34">
+      <c r="N110" s="60">
         <v>61.812199999999997</v>
       </c>
-      <c r="O110" s="34">
+      <c r="O110" s="60">
         <v>59.595999999999997</v>
       </c>
-      <c r="P110" s="34">
+      <c r="P110" s="60">
         <v>66.244699999999995</v>
       </c>
-      <c r="Q110" s="34">
+      <c r="Q110" s="60">
         <v>15488.08691</v>
       </c>
-      <c r="R110" s="4" t="s">
+      <c r="R110" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="S110" s="34">
-        <v>1</v>
-      </c>
-      <c r="T110" s="34">
-        <v>1</v>
-      </c>
-      <c r="V110" s="4" t="s">
+      <c r="S110" s="60">
+        <v>1</v>
+      </c>
+      <c r="T110" s="60">
+        <v>1</v>
+      </c>
+      <c r="V110" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="W110" s="37" t="s">
+      <c r="W110" s="61" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="111" spans="1:30" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="31">
+    <row r="111" spans="1:30" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="53">
         <v>176</v>
       </c>
-      <c r="B111" s="13">
+      <c r="B111" s="54">
         <v>18000</v>
       </c>
-      <c r="C111" s="10">
+      <c r="C111" s="55">
         <v>0.98</v>
       </c>
-      <c r="D111" s="10">
+      <c r="D111" s="55">
         <v>32</v>
       </c>
-      <c r="E111" s="10">
-        <v>5</v>
-      </c>
-      <c r="F111" s="10">
-        <v>2</v>
-      </c>
-      <c r="G111" s="10">
+      <c r="E111" s="55">
+        <v>5</v>
+      </c>
+      <c r="F111" s="55">
+        <v>2</v>
+      </c>
+      <c r="G111" s="55">
         <v>20</v>
       </c>
-      <c r="H111" s="10">
+      <c r="H111" s="55">
         <v>4.7</v>
       </c>
-      <c r="I111" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J111" s="10">
+      <c r="I111" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J111" s="55">
         <v>15</v>
       </c>
-      <c r="K111" s="10">
+      <c r="K111" s="55">
         <v>29</v>
       </c>
-      <c r="L111" s="10">
-        <v>8</v>
-      </c>
-      <c r="M111" s="10">
+      <c r="L111" s="55">
+        <v>8</v>
+      </c>
+      <c r="M111" s="55">
         <v>0.84013180340000004</v>
       </c>
-      <c r="N111" s="10">
+      <c r="N111" s="55">
         <v>83.925399999999996</v>
       </c>
-      <c r="O111" s="10">
+      <c r="O111" s="55">
         <v>86.042400000000001</v>
       </c>
-      <c r="P111" s="10">
+      <c r="P111" s="55">
         <v>79.691500000000005</v>
       </c>
-      <c r="Q111" s="10">
+      <c r="Q111" s="55">
         <v>1681.5981449999999</v>
       </c>
-      <c r="R111" s="9" t="s">
+      <c r="R111" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="S111" s="10">
-        <v>1</v>
-      </c>
-      <c r="T111" s="10">
-        <v>1</v>
-      </c>
-      <c r="U111" s="9">
+      <c r="S111" s="55">
+        <v>1</v>
+      </c>
+      <c r="T111" s="55">
+        <v>1</v>
+      </c>
+      <c r="U111" s="6">
         <v>2875.0443420000001</v>
       </c>
-      <c r="V111" s="9" t="s">
+      <c r="V111" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="W111" s="12"/>
-      <c r="X111" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y111" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z111" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA111" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB111" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC111" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD111" s="9" t="s">
+      <c r="W111" s="57"/>
+      <c r="X111" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y111" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z111" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA111" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB111" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC111" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD111" s="6" t="s">
         <v>198</v>
       </c>
     </row>
@@ -10038,6 +10068,102 @@
       </c>
       <c r="AD134" s="9" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="136" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B138" s="9">
+        <v>5000</v>
+      </c>
+      <c r="C138" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E138" s="9">
+        <v>3</v>
+      </c>
+      <c r="F138" s="9">
+        <v>3</v>
+      </c>
+      <c r="G138" s="9">
+        <v>26</v>
+      </c>
+      <c r="H138" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="I138" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J138" s="9">
+        <v>16</v>
+      </c>
+      <c r="K138" s="9">
+        <v>50</v>
+      </c>
+      <c r="L138" s="9">
+        <v>8</v>
+      </c>
+      <c r="O138" s="9">
+        <v>92.93</v>
+      </c>
+      <c r="P138" s="9">
+        <v>63.47</v>
+      </c>
+      <c r="Q138" s="9">
+        <v>852</v>
+      </c>
+      <c r="R138" s="9">
+        <v>8.3835999999999995</v>
+      </c>
+    </row>
+    <row r="139" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A139" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B139">
+        <v>2000</v>
+      </c>
+      <c r="C139" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E139">
+        <v>2</v>
+      </c>
+      <c r="F139">
+        <v>2</v>
+      </c>
+      <c r="G139">
+        <v>26</v>
+      </c>
+      <c r="H139">
+        <v>2.5</v>
+      </c>
+      <c r="I139" t="s">
+        <v>18</v>
+      </c>
+      <c r="J139">
+        <v>16</v>
+      </c>
+      <c r="K139">
+        <v>50</v>
+      </c>
+      <c r="L139">
+        <v>8</v>
+      </c>
+      <c r="O139">
+        <v>100</v>
+      </c>
+      <c r="P139">
+        <v>100</v>
+      </c>
+      <c r="Q139">
+        <v>343</v>
+      </c>
+      <c r="R139">
+        <v>8.5451999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>